<commit_message>
Big fix of ABS & RBA data sources
</commit_message>
<xml_diff>
--- a/User_Data/ABS/Full_Sheets/634501.xlsx
+++ b/User_Data/ABS/Full_Sheets/634501.xlsx
@@ -17,89 +17,89 @@
     <sheet name="Enquiries" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="A2603039T">Data1!$B$1:$B$10,Data1!$B$11:$B$122</definedName>
-    <definedName name="A2603039T_Data">Data1!$B$11:$B$122</definedName>
-    <definedName name="A2603039T_Latest">Data1!$B$122</definedName>
-    <definedName name="A2603040A">Data1!$K$1:$K$10,Data1!$K$11:$K$122</definedName>
-    <definedName name="A2603040A_Data">Data1!$K$11:$K$122</definedName>
-    <definedName name="A2603040A_Latest">Data1!$K$122</definedName>
-    <definedName name="A2603041C">Data1!$T$1:$T$10,Data1!$T$11:$T$122</definedName>
-    <definedName name="A2603041C_Data">Data1!$T$11:$T$122</definedName>
-    <definedName name="A2603041C_Latest">Data1!$T$122</definedName>
-    <definedName name="A2603609J">Data1!$D$1:$D$10,Data1!$D$11:$D$122</definedName>
-    <definedName name="A2603609J_Data">Data1!$D$11:$D$122</definedName>
-    <definedName name="A2603609J_Latest">Data1!$D$122</definedName>
-    <definedName name="A2603610T">Data1!$M$1:$M$10,Data1!$M$11:$M$122</definedName>
-    <definedName name="A2603610T_Data">Data1!$M$11:$M$122</definedName>
-    <definedName name="A2603610T_Latest">Data1!$M$122</definedName>
-    <definedName name="A2603611V">Data1!$V$1:$V$10,Data1!$V$11:$V$122</definedName>
-    <definedName name="A2603611V_Data">Data1!$V$11:$V$122</definedName>
-    <definedName name="A2603611V_Latest">Data1!$V$122</definedName>
-    <definedName name="A2603989W">Data1!$C$1:$C$10,Data1!$C$11:$C$122</definedName>
-    <definedName name="A2603989W_Data">Data1!$C$11:$C$122</definedName>
-    <definedName name="A2603989W_Latest">Data1!$C$122</definedName>
-    <definedName name="A2603990F">Data1!$L$1:$L$10,Data1!$L$11:$L$122</definedName>
-    <definedName name="A2603990F_Data">Data1!$L$11:$L$122</definedName>
-    <definedName name="A2603990F_Latest">Data1!$L$122</definedName>
-    <definedName name="A2603991J">Data1!$U$1:$U$10,Data1!$U$11:$U$122</definedName>
-    <definedName name="A2603991J_Data">Data1!$U$11:$U$122</definedName>
-    <definedName name="A2603991J_Latest">Data1!$U$122</definedName>
-    <definedName name="A2713846W">Data1!$E$1:$E$10,Data1!$E$11:$E$122</definedName>
-    <definedName name="A2713846W_Data">Data1!$E$11:$E$122</definedName>
-    <definedName name="A2713846W_Latest">Data1!$E$122</definedName>
-    <definedName name="A2713848A">Data1!$H$1:$H$10,Data1!$H$11:$H$122</definedName>
-    <definedName name="A2713848A_Data">Data1!$H$11:$H$122</definedName>
-    <definedName name="A2713848A_Latest">Data1!$H$122</definedName>
-    <definedName name="A2713849C">Data1!$G$1:$G$10,Data1!$G$11:$G$122</definedName>
-    <definedName name="A2713849C_Data">Data1!$G$11:$G$122</definedName>
-    <definedName name="A2713849C_Latest">Data1!$G$122</definedName>
-    <definedName name="A2713851R">Data1!$J$1:$J$10,Data1!$J$11:$J$122</definedName>
-    <definedName name="A2713851R_Data">Data1!$J$11:$J$122</definedName>
-    <definedName name="A2713851R_Latest">Data1!$J$122</definedName>
-    <definedName name="A2713852T">Data1!$F$1:$F$10,Data1!$F$11:$F$122</definedName>
-    <definedName name="A2713852T_Data">Data1!$F$11:$F$122</definedName>
-    <definedName name="A2713852T_Latest">Data1!$F$122</definedName>
-    <definedName name="A2713854W">Data1!$I$1:$I$10,Data1!$I$11:$I$122</definedName>
-    <definedName name="A2713854W_Data">Data1!$I$11:$I$122</definedName>
-    <definedName name="A2713854W_Latest">Data1!$I$122</definedName>
-    <definedName name="A83895308K">Data1!$N$1:$N$10,Data1!$N$11:$N$122</definedName>
-    <definedName name="A83895308K_Data">Data1!$N$11:$N$122</definedName>
-    <definedName name="A83895308K_Latest">Data1!$N$122</definedName>
-    <definedName name="A83895309L">Data1!$W$1:$W$10,Data1!$W$11:$W$122</definedName>
-    <definedName name="A83895309L_Data">Data1!$W$11:$W$122</definedName>
-    <definedName name="A83895309L_Latest">Data1!$W$122</definedName>
-    <definedName name="A83895311X">Data1!$Q$1:$Q$10,Data1!$Q$11:$Q$122</definedName>
-    <definedName name="A83895311X_Data">Data1!$Q$11:$Q$122</definedName>
-    <definedName name="A83895311X_Latest">Data1!$Q$122</definedName>
-    <definedName name="A83895312A">Data1!$Z$1:$Z$10,Data1!$Z$11:$Z$122</definedName>
-    <definedName name="A83895312A_Data">Data1!$Z$11:$Z$122</definedName>
-    <definedName name="A83895312A_Latest">Data1!$Z$122</definedName>
-    <definedName name="A83895332K">Data1!$O$1:$O$10,Data1!$O$11:$O$122</definedName>
-    <definedName name="A83895332K_Data">Data1!$O$11:$O$122</definedName>
-    <definedName name="A83895332K_Latest">Data1!$O$122</definedName>
-    <definedName name="A83895333L">Data1!$X$1:$X$10,Data1!$X$11:$X$122</definedName>
-    <definedName name="A83895333L_Data">Data1!$X$11:$X$122</definedName>
-    <definedName name="A83895333L_Latest">Data1!$X$122</definedName>
-    <definedName name="A83895335T">Data1!$R$1:$R$10,Data1!$R$11:$R$122</definedName>
-    <definedName name="A83895335T_Data">Data1!$R$11:$R$122</definedName>
-    <definedName name="A83895335T_Latest">Data1!$R$122</definedName>
-    <definedName name="A83895336V">Data1!$AA$1:$AA$10,Data1!$AA$11:$AA$122</definedName>
-    <definedName name="A83895336V_Data">Data1!$AA$11:$AA$122</definedName>
-    <definedName name="A83895336V_Latest">Data1!$AA$122</definedName>
-    <definedName name="A83895395V">Data1!$P$1:$P$10,Data1!$P$11:$P$122</definedName>
-    <definedName name="A83895395V_Data">Data1!$P$11:$P$122</definedName>
-    <definedName name="A83895395V_Latest">Data1!$P$122</definedName>
-    <definedName name="A83895396W">Data1!$Y$1:$Y$10,Data1!$Y$11:$Y$122</definedName>
-    <definedName name="A83895396W_Data">Data1!$Y$11:$Y$122</definedName>
-    <definedName name="A83895396W_Latest">Data1!$Y$122</definedName>
-    <definedName name="A83895398A">Data1!$S$1:$S$10,Data1!$S$11:$S$122</definedName>
-    <definedName name="A83895398A_Data">Data1!$S$11:$S$122</definedName>
-    <definedName name="A83895398A_Latest">Data1!$S$122</definedName>
-    <definedName name="A83895399C">Data1!$AB$1:$AB$10,Data1!$AB$11:$AB$122</definedName>
-    <definedName name="A83895399C_Data">Data1!$AB$11:$AB$122</definedName>
-    <definedName name="A83895399C_Latest">Data1!$AB$122</definedName>
-    <definedName name="Date_Range">Data1!$A$2:$A$10,Data1!$A$11:$A$122</definedName>
-    <definedName name="Date_Range_Data">Data1!$A$11:$A$122</definedName>
+    <definedName name="A2603039T">Data1!$B$1:$B$10,Data1!$B$11:$B$123</definedName>
+    <definedName name="A2603039T_Data">Data1!$B$11:$B$123</definedName>
+    <definedName name="A2603039T_Latest">Data1!$B$123</definedName>
+    <definedName name="A2603040A">Data1!$K$1:$K$10,Data1!$K$11:$K$123</definedName>
+    <definedName name="A2603040A_Data">Data1!$K$11:$K$123</definedName>
+    <definedName name="A2603040A_Latest">Data1!$K$123</definedName>
+    <definedName name="A2603041C">Data1!$T$1:$T$10,Data1!$T$11:$T$123</definedName>
+    <definedName name="A2603041C_Data">Data1!$T$11:$T$123</definedName>
+    <definedName name="A2603041C_Latest">Data1!$T$123</definedName>
+    <definedName name="A2603609J">Data1!$D$1:$D$10,Data1!$D$11:$D$123</definedName>
+    <definedName name="A2603609J_Data">Data1!$D$11:$D$123</definedName>
+    <definedName name="A2603609J_Latest">Data1!$D$123</definedName>
+    <definedName name="A2603610T">Data1!$M$1:$M$10,Data1!$M$11:$M$123</definedName>
+    <definedName name="A2603610T_Data">Data1!$M$11:$M$123</definedName>
+    <definedName name="A2603610T_Latest">Data1!$M$123</definedName>
+    <definedName name="A2603611V">Data1!$V$1:$V$10,Data1!$V$11:$V$123</definedName>
+    <definedName name="A2603611V_Data">Data1!$V$11:$V$123</definedName>
+    <definedName name="A2603611V_Latest">Data1!$V$123</definedName>
+    <definedName name="A2603989W">Data1!$C$1:$C$10,Data1!$C$11:$C$123</definedName>
+    <definedName name="A2603989W_Data">Data1!$C$11:$C$123</definedName>
+    <definedName name="A2603989W_Latest">Data1!$C$123</definedName>
+    <definedName name="A2603990F">Data1!$L$1:$L$10,Data1!$L$11:$L$123</definedName>
+    <definedName name="A2603990F_Data">Data1!$L$11:$L$123</definedName>
+    <definedName name="A2603990F_Latest">Data1!$L$123</definedName>
+    <definedName name="A2603991J">Data1!$U$1:$U$10,Data1!$U$11:$U$123</definedName>
+    <definedName name="A2603991J_Data">Data1!$U$11:$U$123</definedName>
+    <definedName name="A2603991J_Latest">Data1!$U$123</definedName>
+    <definedName name="A2713846W">Data1!$E$1:$E$10,Data1!$E$11:$E$123</definedName>
+    <definedName name="A2713846W_Data">Data1!$E$11:$E$123</definedName>
+    <definedName name="A2713846W_Latest">Data1!$E$123</definedName>
+    <definedName name="A2713848A">Data1!$H$1:$H$10,Data1!$H$11:$H$123</definedName>
+    <definedName name="A2713848A_Data">Data1!$H$11:$H$123</definedName>
+    <definedName name="A2713848A_Latest">Data1!$H$123</definedName>
+    <definedName name="A2713849C">Data1!$G$1:$G$10,Data1!$G$11:$G$123</definedName>
+    <definedName name="A2713849C_Data">Data1!$G$11:$G$123</definedName>
+    <definedName name="A2713849C_Latest">Data1!$G$123</definedName>
+    <definedName name="A2713851R">Data1!$J$1:$J$10,Data1!$J$11:$J$123</definedName>
+    <definedName name="A2713851R_Data">Data1!$J$11:$J$123</definedName>
+    <definedName name="A2713851R_Latest">Data1!$J$123</definedName>
+    <definedName name="A2713852T">Data1!$F$1:$F$10,Data1!$F$11:$F$123</definedName>
+    <definedName name="A2713852T_Data">Data1!$F$11:$F$123</definedName>
+    <definedName name="A2713852T_Latest">Data1!$F$123</definedName>
+    <definedName name="A2713854W">Data1!$I$1:$I$10,Data1!$I$11:$I$123</definedName>
+    <definedName name="A2713854W_Data">Data1!$I$11:$I$123</definedName>
+    <definedName name="A2713854W_Latest">Data1!$I$123</definedName>
+    <definedName name="A83895308K">Data1!$N$1:$N$10,Data1!$N$11:$N$123</definedName>
+    <definedName name="A83895308K_Data">Data1!$N$11:$N$123</definedName>
+    <definedName name="A83895308K_Latest">Data1!$N$123</definedName>
+    <definedName name="A83895309L">Data1!$W$1:$W$10,Data1!$W$11:$W$123</definedName>
+    <definedName name="A83895309L_Data">Data1!$W$11:$W$123</definedName>
+    <definedName name="A83895309L_Latest">Data1!$W$123</definedName>
+    <definedName name="A83895311X">Data1!$Q$1:$Q$10,Data1!$Q$11:$Q$123</definedName>
+    <definedName name="A83895311X_Data">Data1!$Q$11:$Q$123</definedName>
+    <definedName name="A83895311X_Latest">Data1!$Q$123</definedName>
+    <definedName name="A83895312A">Data1!$Z$1:$Z$10,Data1!$Z$11:$Z$123</definedName>
+    <definedName name="A83895312A_Data">Data1!$Z$11:$Z$123</definedName>
+    <definedName name="A83895312A_Latest">Data1!$Z$123</definedName>
+    <definedName name="A83895332K">Data1!$O$1:$O$10,Data1!$O$11:$O$123</definedName>
+    <definedName name="A83895332K_Data">Data1!$O$11:$O$123</definedName>
+    <definedName name="A83895332K_Latest">Data1!$O$123</definedName>
+    <definedName name="A83895333L">Data1!$X$1:$X$10,Data1!$X$11:$X$123</definedName>
+    <definedName name="A83895333L_Data">Data1!$X$11:$X$123</definedName>
+    <definedName name="A83895333L_Latest">Data1!$X$123</definedName>
+    <definedName name="A83895335T">Data1!$R$1:$R$10,Data1!$R$11:$R$123</definedName>
+    <definedName name="A83895335T_Data">Data1!$R$11:$R$123</definedName>
+    <definedName name="A83895335T_Latest">Data1!$R$123</definedName>
+    <definedName name="A83895336V">Data1!$AA$1:$AA$10,Data1!$AA$11:$AA$123</definedName>
+    <definedName name="A83895336V_Data">Data1!$AA$11:$AA$123</definedName>
+    <definedName name="A83895336V_Latest">Data1!$AA$123</definedName>
+    <definedName name="A83895395V">Data1!$P$1:$P$10,Data1!$P$11:$P$123</definedName>
+    <definedName name="A83895395V_Data">Data1!$P$11:$P$123</definedName>
+    <definedName name="A83895395V_Latest">Data1!$P$123</definedName>
+    <definedName name="A83895396W">Data1!$Y$1:$Y$10,Data1!$Y$11:$Y$123</definedName>
+    <definedName name="A83895396W_Data">Data1!$Y$11:$Y$123</definedName>
+    <definedName name="A83895396W_Latest">Data1!$Y$123</definedName>
+    <definedName name="A83895398A">Data1!$S$1:$S$10,Data1!$S$11:$S$123</definedName>
+    <definedName name="A83895398A_Data">Data1!$S$11:$S$123</definedName>
+    <definedName name="A83895398A_Latest">Data1!$S$123</definedName>
+    <definedName name="A83895399C">Data1!$AB$1:$AB$10,Data1!$AB$11:$AB$123</definedName>
+    <definedName name="A83895399C_Data">Data1!$AB$11:$AB$123</definedName>
+    <definedName name="A83895399C_Latest">Data1!$AB$123</definedName>
+    <definedName name="Date_Range">Data1!$A$2:$A$10,Data1!$A$11:$A$123</definedName>
+    <definedName name="Date_Range_Data">Data1!$A$11:$A$123</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1871,10 +1871,10 @@
         <v>35674</v>
       </c>
       <c r="G12" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H12" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>24</v>
@@ -1903,10 +1903,10 @@
         <v>35674</v>
       </c>
       <c r="G13" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H13" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I13" s="10" t="s">
         <v>24</v>
@@ -1935,10 +1935,10 @@
         <v>35674</v>
       </c>
       <c r="G14" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H14" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>24</v>
@@ -1967,10 +1967,10 @@
         <v>35674</v>
       </c>
       <c r="G15" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H15" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I15" s="10" t="s">
         <v>24</v>
@@ -1999,10 +1999,10 @@
         <v>35674</v>
       </c>
       <c r="G16" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H16" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I16" s="10" t="s">
         <v>24</v>
@@ -2031,10 +2031,10 @@
         <v>35674</v>
       </c>
       <c r="G17" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H17" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I17" s="10" t="s">
         <v>24</v>
@@ -2063,10 +2063,10 @@
         <v>35674</v>
       </c>
       <c r="G18" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H18" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I18" s="10" t="s">
         <v>24</v>
@@ -2095,10 +2095,10 @@
         <v>35674</v>
       </c>
       <c r="G19" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H19" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I19" s="10" t="s">
         <v>24</v>
@@ -2127,10 +2127,10 @@
         <v>35674</v>
       </c>
       <c r="G20" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H20" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I20" s="10" t="s">
         <v>24</v>
@@ -2159,10 +2159,10 @@
         <v>35674</v>
       </c>
       <c r="G21" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H21" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I21" s="10" t="s">
         <v>39</v>
@@ -2191,10 +2191,10 @@
         <v>35674</v>
       </c>
       <c r="G22" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H22" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I22" s="10" t="s">
         <v>39</v>
@@ -2223,10 +2223,10 @@
         <v>35674</v>
       </c>
       <c r="G23" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H23" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I23" s="10" t="s">
         <v>39</v>
@@ -2255,10 +2255,10 @@
         <v>35674</v>
       </c>
       <c r="G24" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H24" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I24" s="10" t="s">
         <v>39</v>
@@ -2287,10 +2287,10 @@
         <v>35674</v>
       </c>
       <c r="G25" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H25" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I25" s="10" t="s">
         <v>39</v>
@@ -2319,10 +2319,10 @@
         <v>35674</v>
       </c>
       <c r="G26" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H26" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I26" s="10" t="s">
         <v>39</v>
@@ -2351,10 +2351,10 @@
         <v>35674</v>
       </c>
       <c r="G27" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H27" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I27" s="10" t="s">
         <v>39</v>
@@ -2383,10 +2383,10 @@
         <v>35674</v>
       </c>
       <c r="G28" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H28" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I28" s="10" t="s">
         <v>39</v>
@@ -2415,10 +2415,10 @@
         <v>35674</v>
       </c>
       <c r="G29" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H29" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I29" s="10" t="s">
         <v>39</v>
@@ -2447,10 +2447,10 @@
         <v>35674</v>
       </c>
       <c r="G30" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H30" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I30" s="10" t="s">
         <v>39</v>
@@ -2479,10 +2479,10 @@
         <v>35674</v>
       </c>
       <c r="G31" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H31" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I31" s="10" t="s">
         <v>39</v>
@@ -2511,10 +2511,10 @@
         <v>35674</v>
       </c>
       <c r="G32" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H32" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I32" s="10" t="s">
         <v>39</v>
@@ -2543,10 +2543,10 @@
         <v>35674</v>
       </c>
       <c r="G33" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H33" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I33" s="10" t="s">
         <v>39</v>
@@ -2575,10 +2575,10 @@
         <v>35674</v>
       </c>
       <c r="G34" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H34" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I34" s="10" t="s">
         <v>39</v>
@@ -2607,10 +2607,10 @@
         <v>35674</v>
       </c>
       <c r="G35" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H35" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I35" s="10" t="s">
         <v>39</v>
@@ -2639,10 +2639,10 @@
         <v>35674</v>
       </c>
       <c r="G36" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H36" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I36" s="10" t="s">
         <v>39</v>
@@ -2671,10 +2671,10 @@
         <v>35674</v>
       </c>
       <c r="G37" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H37" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I37" s="10" t="s">
         <v>39</v>
@@ -2703,10 +2703,10 @@
         <v>35674</v>
       </c>
       <c r="G38" s="9">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H38" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I38" s="10" t="s">
         <v>39</v>
@@ -2768,7 +2768,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB122"/>
+  <dimension ref="A1:AB123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
@@ -3386,85 +3386,85 @@
         <v>21</v>
       </c>
       <c r="B8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="C8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="D8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="E8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="F8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="G8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="H8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="I8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="J8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="K8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="L8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="M8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="N8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="O8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="P8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="Q8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="R8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="S8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="T8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="U8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="V8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="W8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="X8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="Y8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="Z8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="AA8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
       <c r="AB8" s="6">
-        <v>45809</v>
+        <v>45901</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
@@ -3472,85 +3472,85 @@
         <v>22</v>
       </c>
       <c r="B9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="K9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="L9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="M9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="N9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="P9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Q9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="R9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="S9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="T9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="U9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="V9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="W9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="X9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Y9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Z9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AA9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AB9" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
@@ -11825,7 +11825,7 @@
         <v>140.69999999999999</v>
       </c>
       <c r="G107" s="8">
-        <v>137.4</v>
+        <v>137.5</v>
       </c>
       <c r="H107" s="8">
         <v>136.6</v>
@@ -11852,7 +11852,7 @@
         <v>0.6</v>
       </c>
       <c r="P107" s="8">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="Q107" s="8">
         <v>0.6</v>
@@ -12223,7 +12223,7 @@
         <v>2.4</v>
       </c>
       <c r="Y111" s="8">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="Z111" s="8">
         <v>3.2</v>
@@ -12255,7 +12255,7 @@
         <v>145.19999999999999</v>
       </c>
       <c r="G112" s="8">
-        <v>143.1</v>
+        <v>143</v>
       </c>
       <c r="H112" s="8">
         <v>142.4</v>
@@ -12282,7 +12282,7 @@
         <v>0.8</v>
       </c>
       <c r="P112" s="8">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="Q112" s="8">
         <v>1</v>
@@ -12309,7 +12309,7 @@
         <v>2.5</v>
       </c>
       <c r="Y112" s="8">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="Z112" s="8">
         <v>3.6</v>
@@ -12368,7 +12368,7 @@
         <v>0.9</v>
       </c>
       <c r="P113" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="Q113" s="8">
         <v>0.9</v>
@@ -12424,7 +12424,7 @@
         <v>145</v>
       </c>
       <c r="F114" s="8">
-        <v>147.6</v>
+        <v>147.69999999999999</v>
       </c>
       <c r="G114" s="8">
         <v>145.6</v>
@@ -12516,7 +12516,7 @@
         <v>147.5</v>
       </c>
       <c r="H115" s="8">
-        <v>146.9</v>
+        <v>146.80000000000001</v>
       </c>
       <c r="I115" s="8">
         <v>149.4</v>
@@ -12537,13 +12537,13 @@
         <v>1.4</v>
       </c>
       <c r="O115" s="8">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="P115" s="8">
         <v>1.3</v>
       </c>
       <c r="Q115" s="8">
-        <v>1.2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="R115" s="8">
         <v>1.1000000000000001</v>
@@ -12570,7 +12570,7 @@
         <v>4</v>
       </c>
       <c r="Z115" s="8">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="AA115" s="8">
         <v>3.7</v>
@@ -12629,7 +12629,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="Q116" s="8">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="R116" s="8">
         <v>1</v>
@@ -12653,7 +12653,7 @@
         <v>4.3</v>
       </c>
       <c r="Y116" s="8">
-        <v>4.2</v>
+        <v>4.3</v>
       </c>
       <c r="Z116" s="8">
         <v>4.2</v>
@@ -12768,7 +12768,7 @@
         <v>150.9</v>
       </c>
       <c r="F118" s="8">
-        <v>153.4</v>
+        <v>153.5</v>
       </c>
       <c r="G118" s="8">
         <v>151.5</v>
@@ -12795,7 +12795,7 @@
         <v>0.8</v>
       </c>
       <c r="O118" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="P118" s="8">
         <v>0.9</v>
@@ -12863,7 +12863,7 @@
         <v>152.1</v>
       </c>
       <c r="I119" s="8">
-        <v>154.6</v>
+        <v>154.5</v>
       </c>
       <c r="J119" s="8">
         <v>152.69999999999999</v>
@@ -12881,7 +12881,7 @@
         <v>0.9</v>
       </c>
       <c r="O119" s="8">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="P119" s="8">
         <v>0.8</v>
@@ -12890,7 +12890,7 @@
         <v>0.8</v>
       </c>
       <c r="R119" s="8">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="S119" s="8">
         <v>0.8</v>
@@ -12914,10 +12914,10 @@
         <v>3.5</v>
       </c>
       <c r="Z119" s="8">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="AA119" s="8">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="AB119" s="8">
         <v>3.6</v>
@@ -12940,7 +12940,7 @@
         <v>153.30000000000001</v>
       </c>
       <c r="F120" s="8">
-        <v>155.80000000000001</v>
+        <v>155.69999999999999</v>
       </c>
       <c r="G120" s="8">
         <v>153.9</v>
@@ -12949,7 +12949,7 @@
         <v>153.4</v>
       </c>
       <c r="I120" s="8">
-        <v>156</v>
+        <v>155.9</v>
       </c>
       <c r="J120" s="8">
         <v>154</v>
@@ -12967,7 +12967,7 @@
         <v>0.7</v>
       </c>
       <c r="O120" s="8">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="P120" s="8">
         <v>0.8</v>
@@ -12994,7 +12994,7 @@
         <v>3.3</v>
       </c>
       <c r="X120" s="8">
-        <v>2.9</v>
+        <v>2.8</v>
       </c>
       <c r="Y120" s="8">
         <v>3.2</v>
@@ -13003,7 +13003,7 @@
         <v>3.4</v>
       </c>
       <c r="AA120" s="8">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="AB120" s="8">
         <v>3.4</v>
@@ -13029,7 +13029,7 @@
         <v>157.5</v>
       </c>
       <c r="G121" s="8">
-        <v>155.30000000000001</v>
+        <v>155.4</v>
       </c>
       <c r="H121" s="8">
         <v>154.69999999999999</v>
@@ -13053,16 +13053,16 @@
         <v>0.9</v>
       </c>
       <c r="O121" s="8">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="P121" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="Q121" s="8">
         <v>0.8</v>
       </c>
       <c r="R121" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="S121" s="8">
         <v>0.8</v>
@@ -13083,7 +13083,7 @@
         <v>3.6</v>
       </c>
       <c r="Y121" s="8">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="Z121" s="8">
         <v>3.3</v>
@@ -13112,16 +13112,16 @@
         <v>156</v>
       </c>
       <c r="F122" s="8">
-        <v>159</v>
+        <v>159.1</v>
       </c>
       <c r="G122" s="8">
-        <v>156.6</v>
+        <v>156.69999999999999</v>
       </c>
       <c r="H122" s="8">
         <v>155.9</v>
       </c>
       <c r="I122" s="8">
-        <v>158.9</v>
+        <v>159</v>
       </c>
       <c r="J122" s="8">
         <v>156.6</v>
@@ -13166,7 +13166,7 @@
         <v>3.4</v>
       </c>
       <c r="X122" s="8">
-        <v>3.7</v>
+        <v>3.6</v>
       </c>
       <c r="Y122" s="8">
         <v>3.4</v>
@@ -13175,9 +13175,95 @@
         <v>3.3</v>
       </c>
       <c r="AA122" s="8">
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
       <c r="AB122" s="8">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A123" s="9">
+        <v>45901</v>
+      </c>
+      <c r="B123" s="8">
+        <v>157.6</v>
+      </c>
+      <c r="C123" s="8">
+        <v>160.5</v>
+      </c>
+      <c r="D123" s="8">
+        <v>158.30000000000001</v>
+      </c>
+      <c r="E123" s="8">
+        <v>157.1</v>
+      </c>
+      <c r="F123" s="8">
+        <v>160.5</v>
+      </c>
+      <c r="G123" s="8">
+        <v>157.9</v>
+      </c>
+      <c r="H123" s="8">
+        <v>157.19999999999999</v>
+      </c>
+      <c r="I123" s="8">
+        <v>160.6</v>
+      </c>
+      <c r="J123" s="8">
+        <v>157.9</v>
+      </c>
+      <c r="K123" s="8">
+        <v>1.4</v>
+      </c>
+      <c r="L123" s="8">
+        <v>1</v>
+      </c>
+      <c r="M123" s="8">
+        <v>1.3</v>
+      </c>
+      <c r="N123" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="O123" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="P123" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="Q123" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="R123" s="8">
+        <v>1</v>
+      </c>
+      <c r="S123" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="T123" s="8">
+        <v>3.3</v>
+      </c>
+      <c r="U123" s="8">
+        <v>3.8</v>
+      </c>
+      <c r="V123" s="8">
+        <v>3.4</v>
+      </c>
+      <c r="W123" s="8">
+        <v>3.2</v>
+      </c>
+      <c r="X123" s="8">
+        <v>3.8</v>
+      </c>
+      <c r="Y123" s="8">
+        <v>3.4</v>
+      </c>
+      <c r="Z123" s="8">
+        <v>3.4</v>
+      </c>
+      <c r="AA123" s="8">
+        <v>3.9</v>
+      </c>
+      <c r="AB123" s="8">
         <v>3.4</v>
       </c>
     </row>

</xml_diff>